<commit_message>
Update DatabaseTable, DatabaseData, Improved ERD
</commit_message>
<xml_diff>
--- a/VectorDataInExcel.xlsx
+++ b/VectorDataInExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Database\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{25ACCE83-8715-42FB-9CCD-0E14EBF74E55}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{0C4B9539-F4EF-4586-BA83-0A829C3719DB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7DCE2BE0-953A-4365-ADEC-B2ECAC53B523}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="181">
   <si>
     <t>Column1</t>
   </si>
@@ -1029,14 +1029,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B6293B-0427-4036-815C-5BCCB8EDF1A2}">
   <dimension ref="A1:BL74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="10" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="8" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" customWidth="1"/>
     <col min="12" max="38" width="15.7109375" customWidth="1"/>
     <col min="39" max="39" width="22.42578125" customWidth="1"/>
@@ -2160,9 +2166,6 @@
       <c r="B49" t="s">
         <v>119</v>
       </c>
-      <c r="C49" t="s">
-        <v>120</v>
-      </c>
       <c r="D49" t="s">
         <v>121</v>
       </c>
@@ -2272,8 +2275,8 @@
       <c r="A54" t="s">
         <v>144</v>
       </c>
-      <c r="B54" t="s">
-        <v>145</v>
+      <c r="B54">
+        <v>8.9610180002248999E+19</v>
       </c>
       <c r="C54" t="s">
         <v>146</v>
@@ -2287,8 +2290,8 @@
       <c r="F54" t="s">
         <v>148</v>
       </c>
-      <c r="G54" t="s">
-        <v>149</v>
+      <c r="G54">
+        <v>8.9610180002248999E+19</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>